<commit_message>
Societal test evaluation -work in progress
</commit_message>
<xml_diff>
--- a/src/dataset/template_subjects.xlsx
+++ b/src/dataset/template_subjects.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>target</t>
   </si>
@@ -103,17 +103,20 @@
     <t>man</t>
   </si>
   <si>
-    <t>women</t>
-  </si>
-  <si>
-    <t>men</t>
+    <t>target4</t>
+  </si>
+  <si>
+    <t>her</t>
+  </si>
+  <si>
+    <t>him</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -129,6 +132,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -203,6 +211,15 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,14 +515,14 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -513,10 +530,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -524,10 +541,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -535,21 +552,21 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -557,10 +574,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
@@ -568,10 +585,21 @@
         <v>25</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>31</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>